<commit_message>
ADD: Phase1.tex and .pdf
</commit_message>
<xml_diff>
--- a/ProjManag/Budget.xlsx
+++ b/ProjManag/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zemiguel/Dropbox/LPI1-PI/GestaoProj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zemiguel/Documents/Univ/MI_Electro/Sem6/LPI2/PI/github/ProjManag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC1A3FB-E714-B44F-AF52-2F2C30E7E479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94B6B8C-4A60-8149-9A1B-47E0BD16D997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="16000" xr2:uid="{06AB5143-CC34-3E48-939D-F6D9ED0C8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{06AB5143-CC34-3E48-939D-F6D9ED0C8206}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -105,13 +105,79 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>In Stock</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero</t>
+  </si>
+  <si>
+    <t>Pi Hub</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Computational Platform</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero Camera</t>
+  </si>
+  <si>
+    <t>yes?</t>
+  </si>
+  <si>
+    <t>https://www.botnroll.com/pt/bases/2151--kit-iniciacao-para-robo-mecanica-.html</t>
+  </si>
+  <si>
+    <t>Car platform</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero Power supply</t>
+  </si>
+  <si>
+    <t>Worten</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero SD Card (8GB)</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>STM32</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Car Rechargeable Battery</t>
+  </si>
+  <si>
+    <t>Rechargeable Battery system</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Car HW</t>
+  </si>
+  <si>
+    <t>Lighting system (2 mini headlights)</t>
+  </si>
+  <si>
+    <t>Odometric Sensors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,8 +193,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +212,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,10 +255,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -180,8 +267,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -195,6 +292,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>653092</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51943A6A-0362-7946-9DFA-A59D8BB58674}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8013700" y="3352800"/>
+          <a:ext cx="2773992" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,20 +640,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C533EC-CF42-BF42-839F-E3EFB3C91417}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -535,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -549,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -563,7 +709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -577,7 +723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -591,7 +737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -605,7 +751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -619,7 +765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -633,7 +779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -647,7 +793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -661,20 +807,243 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="6">
         <f>SUM(B2:B11)</f>
         <v>96.54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="10" customFormat="1">
+      <c r="A16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="8">
+        <v>15.98</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1">
+      <c r="A17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="9">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1">
+      <c r="A18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="10" customFormat="1">
+      <c r="A19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="9">
+        <v>6</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="13" customFormat="1">
+      <c r="A20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="11">
+        <v>20</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="13" customFormat="1">
+      <c r="A21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="11">
+        <v>5</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="13" customFormat="1">
+      <c r="A22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="13" customFormat="1">
+      <c r="A23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" s="13" customFormat="1">
+      <c r="A24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" s="13" customFormat="1">
+      <c r="A25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" s="13" customFormat="1">
+      <c r="A26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="11">
+        <v>27</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="15" customFormat="1">
+      <c r="A27" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="14">
+        <v>1</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
     <sortCondition ref="D2:D11"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="C20" r:id="rId1" xr:uid="{B0DAB612-CE2B-C342-A270-8B92C55A8BC8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FINAL: 20 CRLH!!! ;D
</commit_message>
<xml_diff>
--- a/ProjManag/Budget.xlsx
+++ b/ProjManag/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zemiguel/Documents/Univ/MI_Electro/Sem6/LPI2/PI/github/ProjManag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F85D2AC-F1BF-ED46-A6CD-28C0F3BB6448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A34FC83-7CAE-074B-8D5A-693EA739D98A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{06AB5143-CC34-3E48-939D-F6D9ED0C8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{06AB5143-CC34-3E48-939D-F6D9ED0C8206}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -110,9 +110,6 @@
     <t>In Stock</t>
   </si>
   <si>
-    <t>Raspberry Pi Zero</t>
-  </si>
-  <si>
     <t>Pi Hub</t>
   </si>
   <si>
@@ -122,12 +119,6 @@
     <t>Computational Platform</t>
   </si>
   <si>
-    <t>Raspberry Pi Zero Camera</t>
-  </si>
-  <si>
-    <t>yes?</t>
-  </si>
-  <si>
     <t>https://www.botnroll.com/pt/bases/2151--kit-iniciacao-para-robo-mecanica-.html</t>
   </si>
   <si>
@@ -137,43 +128,34 @@
     <t>no</t>
   </si>
   <si>
-    <t>Raspberry Pi Zero Power supply</t>
-  </si>
-  <si>
-    <t>Worten</t>
-  </si>
-  <si>
-    <t>Raspberry Pi Zero SD Card (8GB)</t>
-  </si>
-  <si>
     <t>Smartphone</t>
   </si>
   <si>
-    <t>STM32</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
     <t>Car Rechargeable Battery</t>
   </si>
   <si>
-    <t>Rechargeable Battery system</t>
-  </si>
-  <si>
-    <t>Buzzer</t>
-  </si>
-  <si>
     <t>Car HW</t>
   </si>
   <si>
-    <t>Lighting system (2 mini headlights)</t>
-  </si>
-  <si>
     <t>Odometric Sensors</t>
   </si>
   <si>
-    <t>Smartphone (RAM=?, Storage=?, SO=?)</t>
+    <t>Unit cost (€)</t>
+  </si>
+  <si>
+    <t>Total cost (€)</t>
+  </si>
+  <si>
+    <t>Navigation Subsystem</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Remote Vision susbsystem</t>
   </si>
 </sst>
 </file>
@@ -262,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -279,6 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -301,16 +284,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>444722</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>153588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>653092</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>742213</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>64689</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -333,8 +316,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8013700" y="3352800"/>
-          <a:ext cx="2773992" cy="2146300"/>
+          <a:off x="9579810" y="554641"/>
+          <a:ext cx="2770649" cy="2116890"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -643,20 +626,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C533EC-CF42-BF42-839F-E3EFB3C91417}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -684,7 +667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -698,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -712,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -726,7 +709,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -740,7 +723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -754,7 +737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -768,7 +751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -782,7 +765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -796,7 +779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -810,7 +793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -819,12 +802,12 @@
         <v>96.54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>2</v>
@@ -833,209 +816,210 @@
         <v>18</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8">
+        <v>5</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="8">
-        <v>15.98</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="D16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="10">
+        <f>B16*E16</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="9">
+        <v>20</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="9">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="E17" s="9">
         <v>1</v>
       </c>
       <c r="F17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" ref="G17:G22" si="0">B17*E17</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="11">
+        <v>20</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+      <c r="G18" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="11">
+        <v>5</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9" t="s">
+      <c r="E19" s="11">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="11">
+        <v>7.95</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="11">
+        <v>9</v>
+      </c>
+      <c r="G20" s="10">
+        <f t="shared" si="0"/>
+        <v>71.55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="11">
+        <v>27</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="G21" s="10">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="14">
         <v>1</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="9">
-        <v>6</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="9">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="11">
-        <v>20</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="11">
-        <v>1</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="11">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="11">
-        <v>27</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="11">
-        <v>1</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="14">
-        <v>1</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>27</v>
+      <c r="F22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="16">
+        <f>SUM(G16:G22)</f>
+        <v>148.55000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="G25">
+        <f>G23*D25</f>
+        <v>1485500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>250</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <f>D26*E26*F26</f>
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <f>SUM(G25+G26)</f>
+        <v>1503000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <f>G27/10000</f>
+        <v>150.30000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1043,7 +1027,7 @@
     <sortCondition ref="D2:D11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C20" r:id="rId1" xr:uid="{B0DAB612-CE2B-C342-A270-8B92C55A8BC8}"/>
+    <hyperlink ref="C18" r:id="rId1" xr:uid="{B0DAB612-CE2B-C342-A270-8B92C55A8BC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>